<commit_message>
Avance 01 - Cronograma
Avance las correcciones (fechas e hitos) hasta la quincena de noviembre
</commit_message>
<xml_diff>
--- a/desarrollo/SIC/Documentos/PPSIC.xlsx
+++ b/desarrollo/SIC/Documentos/PPSIC.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASSI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PracticandoGit02\Tecnalogia\desarrollo\SIC\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBD6EE6-5D04-4690-9BE8-273384204FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Revisado" sheetId="3" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="268">
   <si>
     <t>Duración</t>
   </si>
@@ -858,12 +866,69 @@
       <t>Auditor</t>
     </r>
   </si>
+  <si>
+    <t>Aplicación web para el control de ventas</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Hito 01 - Plan de viabilidad del proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Hito 02 -  Acta de constitución</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Hito 03 - Documento de especificación de requisitos (ERS - IEEE_830)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Diseño detallado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Diseño componentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Diseño de las interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Diseño de la base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Diseño de los servicios o transacciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Diseño de UX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Hito 04 - Documento de arquitectura de software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Hito 05 - Plan de desarrollo completo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Hito 06 - Prueba de integración completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Hito 07 - Documento del plan de pruebas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Hito 08 - Documentación de ayuda completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Hito 09 - Despliegue completo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Hito 09 - Revisión de post implementación completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Hito 10 - Documento del desarrollo de software completa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -940,8 +1005,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="5"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -966,8 +1100,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1123,11 +1275,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1260,6 +1447,89 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1541,14 +1811,1291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F305-AFDE-4E74-BF64-DC1BF3E91720}">
+  <dimension ref="A1:F92"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="109.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" style="57" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" style="58" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="59" customWidth="1"/>
+    <col min="6" max="16384" width="109.42578125" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="72"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>250</v>
+      </c>
+      <c r="E3" s="64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="50">
+        <v>1</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="51"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="67">
+        <v>43739</v>
+      </c>
+      <c r="D7" s="67">
+        <v>43741</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="67">
+        <v>43741</v>
+      </c>
+      <c r="D8" s="67">
+        <v>43745</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="50">
+        <v>1.2</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="67">
+        <v>43745</v>
+      </c>
+      <c r="D11" s="67">
+        <v>43747</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="67">
+        <v>43747</v>
+      </c>
+      <c r="D12" s="67">
+        <v>43749</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="67">
+        <v>43749</v>
+      </c>
+      <c r="D13" s="67">
+        <v>43751</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="67">
+        <v>43751</v>
+      </c>
+      <c r="D14" s="67">
+        <v>43753</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
+    </row>
+    <row r="16" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="54"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50">
+        <v>1.3</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="67">
+        <v>43753</v>
+      </c>
+      <c r="D18" s="67">
+        <v>43759</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="67">
+        <v>43759</v>
+      </c>
+      <c r="D19" s="67">
+        <v>43765</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="67">
+        <v>43765</v>
+      </c>
+      <c r="D20" s="67">
+        <v>43768</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="67">
+        <v>43768</v>
+      </c>
+      <c r="D21" s="67">
+        <v>43771</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="46">
+        <f>D21-C21</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="71"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="50">
+        <v>2</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="50">
+        <v>2.1</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="67">
+        <v>43771</v>
+      </c>
+      <c r="D25" s="67">
+        <v>43774</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="67">
+        <v>43774</v>
+      </c>
+      <c r="D26" s="67">
+        <v>43776</v>
+      </c>
+      <c r="E26" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="67">
+        <v>43776</v>
+      </c>
+      <c r="D27" s="67">
+        <v>43778</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="67">
+        <v>43778</v>
+      </c>
+      <c r="D29" s="67">
+        <v>43780</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" s="67">
+        <v>43782</v>
+      </c>
+      <c r="D30" s="67">
+        <v>43784</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="67">
+        <v>43782</v>
+      </c>
+      <c r="D31" s="67">
+        <v>43784</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="C32" s="67">
+        <v>43782</v>
+      </c>
+      <c r="D32" s="67">
+        <v>43784</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>259</v>
+      </c>
+      <c r="C33" s="67">
+        <v>43784</v>
+      </c>
+      <c r="D33" s="67">
+        <v>43786</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="71"/>
+    </row>
+    <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="50">
+        <v>3</v>
+      </c>
+      <c r="B35" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="50">
+        <v>3.1</v>
+      </c>
+      <c r="B36" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="B43" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="71"/>
+    </row>
+    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="50">
+        <v>4</v>
+      </c>
+      <c r="B51" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="50">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B52" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="50">
+        <v>4.2</v>
+      </c>
+      <c r="B58" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="54"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="54"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="69" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="70"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="71"/>
+    </row>
+    <row r="64" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="50">
+        <v>4.3</v>
+      </c>
+      <c r="B64" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="54"/>
+      <c r="D65" s="54"/>
+      <c r="E65" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="54"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="54"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="54"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="50">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B70" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" s="54"/>
+      <c r="D74" s="54"/>
+      <c r="E74" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
+      <c r="E75" s="54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="C76" s="70"/>
+      <c r="D76" s="70"/>
+      <c r="E76" s="71"/>
+    </row>
+    <row r="77" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="50">
+        <v>5</v>
+      </c>
+      <c r="B77" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="61"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="50">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B78" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="54"/>
+      <c r="D79" s="54"/>
+      <c r="E79" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="C80" s="54"/>
+      <c r="D80" s="54"/>
+      <c r="E80" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" s="54"/>
+      <c r="D81" s="54"/>
+      <c r="E81" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="54"/>
+      <c r="D82" s="54"/>
+      <c r="E82" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="C83" s="70"/>
+      <c r="D83" s="70"/>
+      <c r="E83" s="71"/>
+    </row>
+    <row r="84" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="50">
+        <v>6</v>
+      </c>
+      <c r="B84" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="50">
+        <v>6.1</v>
+      </c>
+      <c r="B85" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" s="66"/>
+      <c r="D85" s="66"/>
+      <c r="E85" s="66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86" s="54"/>
+      <c r="D86" s="54"/>
+      <c r="E86" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="54"/>
+      <c r="D87" s="54"/>
+      <c r="E87" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="C88" s="54"/>
+      <c r="D88" s="54"/>
+      <c r="E88" s="54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="50">
+        <v>6.3</v>
+      </c>
+      <c r="B89" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89" s="66"/>
+      <c r="D89" s="66"/>
+      <c r="E89" s="66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90" s="54"/>
+      <c r="D90" s="54"/>
+      <c r="E90" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B91" s="69" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" s="70"/>
+      <c r="D91" s="70"/>
+      <c r="E91" s="71"/>
+    </row>
+    <row r="92" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" s="69" t="s">
+        <v>267</v>
+      </c>
+      <c r="C92" s="70"/>
+      <c r="D92" s="70"/>
+      <c r="E92" s="71"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B91:E91"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B50:E50"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.5703125" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2194,15 +3741,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="109.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="109.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" style="13" customWidth="1"/>

</xml_diff>

<commit_message>
Creación de carpetas para Hitos
</commit_message>
<xml_diff>
--- a/desarrollo/SIC/Documentos/PPSIC.xlsx
+++ b/desarrollo/SIC/Documentos/PPSIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PracticandoGit02\Tecnalogia\desarrollo\SIC\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D78F053-5710-458E-8120-8B587ECB3D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF3BBD2-7D14-4BE2-8697-B85D2A90CE86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -921,13 +921,13 @@
     <t xml:space="preserve">       Hito 05 - Desarrollo completo</t>
   </si>
   <si>
-    <t xml:space="preserve">       Hito 06 - Documento de pruebas</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Hito 07 - Manuales</t>
   </si>
   <si>
     <t xml:space="preserve">      Hito 08 - Post implementación completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Hito 06 - Pruebas</t>
   </si>
 </sst>
 </file>
@@ -1470,6 +1470,9 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1523,9 +1526,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1809,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F305-AFDE-4E74-BF64-DC1BF3E91720}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="109.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1823,13 +1823,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
@@ -1932,12 +1932,12 @@
     </row>
     <row r="10" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
     </row>
     <row r="11" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -2027,12 +2027,12 @@
     </row>
     <row r="17" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
     </row>
     <row r="18" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
@@ -2111,12 +2111,12 @@
     </row>
     <row r="23" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38"/>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="56" t="s">
         <v>263</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58"/>
     </row>
     <row r="24" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
@@ -2130,7 +2130,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="50" t="s">
         <v>30</v>
       </c>
@@ -2171,7 +2171,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="50" t="s">
         <v>251</v>
       </c>
@@ -2258,12 +2258,12 @@
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38"/>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="58"/>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
@@ -2432,12 +2432,12 @@
     </row>
     <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="38"/>
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="56" t="s">
         <v>266</v>
       </c>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="58"/>
     </row>
     <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="36"/>
@@ -2705,12 +2705,12 @@
     </row>
     <row r="75" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="38"/>
-      <c r="B75" s="55" t="s">
-        <v>267</v>
-      </c>
-      <c r="C75" s="56"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="57"/>
+      <c r="B75" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="58"/>
     </row>
     <row r="76" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="36"/>
@@ -2780,12 +2780,12 @@
     </row>
     <row r="82" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="38"/>
-      <c r="B82" s="55" t="s">
-        <v>268</v>
-      </c>
-      <c r="C82" s="56"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="57"/>
+      <c r="B82" s="56" t="s">
+        <v>267</v>
+      </c>
+      <c r="C82" s="57"/>
+      <c r="D82" s="57"/>
+      <c r="E82" s="58"/>
     </row>
     <row r="83" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="36"/>
@@ -2866,24 +2866,24 @@
     </row>
     <row r="90" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="38"/>
-      <c r="B90" s="55" t="s">
-        <v>269</v>
-      </c>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="57"/>
+      <c r="B90" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B90:E90"/>
     <mergeCell ref="B50:E50"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B90:E90"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2906,11 +2906,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3009,10 +3009,10 @@
       <c r="A13" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="65" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3020,8 +3020,8 @@
       <c r="A14" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
     </row>
     <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
@@ -3144,17 +3144,17 @@
       <c r="A26" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="69"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="70"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
@@ -3487,10 +3487,10 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="59" t="s">
+      <c r="A60" s="60" t="s">
         <v>207</v>
       </c>
-      <c r="B60" s="59" t="s">
+      <c r="B60" s="60" t="s">
         <v>176</v>
       </c>
       <c r="C60" s="28" t="s">
@@ -3498,22 +3498,22 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="60"/>
-      <c r="B61" s="60"/>
+      <c r="A61" s="61"/>
+      <c r="B61" s="61"/>
       <c r="C61" s="28" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="60"/>
-      <c r="B62" s="60"/>
+      <c r="A62" s="61"/>
+      <c r="B62" s="61"/>
       <c r="C62" s="28" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="61"/>
-      <c r="B63" s="61"/>
+      <c r="A63" s="62"/>
+      <c r="B63" s="62"/>
       <c r="C63" s="29" t="s">
         <v>191</v>
       </c>
@@ -3561,12 +3561,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73"/>
     </row>
     <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
Creación de plantillas de documentos
Creación de los entragables en cada repositorio de los hitos
</commit_message>
<xml_diff>
--- a/desarrollo/SIC/Documentos/PPSIC.xlsx
+++ b/desarrollo/SIC/Documentos/PPSIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PracticandoGit02\Tecnalogia\desarrollo\SIC\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF3BBD2-7D14-4BE2-8697-B85D2A90CE86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E54F22-CF6E-4DCA-8A0C-F27104EBDAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1809,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F305-AFDE-4E74-BF64-DC1BF3E91720}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="109.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>